<commit_message>
began to write the docu
</commit_message>
<xml_diff>
--- a/Zeitplan/Marvin_AudioAnlage_ZeitplanAnforderungenBoM_NoraHueppi_20250313.xlsx
+++ b/Zeitplan/Marvin_AudioAnlage_ZeitplanAnforderungenBoM_NoraHueppi_20250313.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\data\Schule\BuP\5_Semester\Marvin\MarvinProject\6_Semester\documentation\Zeitplan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\OneDrive\Berufsschule\BuP\6_Semester\Marvin\Marvin_docu\Zeitplan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A997A25-6CB1-489F-B724-D066958B91A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD75A714-3D3B-4B2E-9B38-0F1ACBE33AF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5CC49039-70A6-4A49-B6FD-A7C35AB692E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplan" sheetId="4" r:id="rId1"/>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Status</t>
-  </si>
-  <si>
-    <t>UNFUNKTIONALE ANFORDERUNGEN</t>
   </si>
   <si>
     <t>Der Sensor soll selbst aufgenommene Audiosignale auslösen</t>
@@ -439,6 +436,9 @@
   <si>
     <t>Leistungsaufgahme</t>
   </si>
+  <si>
+    <t>NICHT FUNKTIONALE ANFORDERUNGEN</t>
+  </si>
 </sst>
 </file>
 
@@ -1312,7 +1312,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1442,14 +1442,8 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1460,20 +1454,32 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1481,44 +1487,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1541,26 +1517,50 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1589,7 +1589,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2285,25 +2284,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730C7784-EAA3-4F75-A441-9364A27E8BAB}">
   <dimension ref="A1:XFD37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="BH42" sqref="BH42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="135" width="4" customWidth="1"/>
-    <col min="136" max="158" width="10.85546875" customWidth="1"/>
-    <col min="16384" max="16384" width="10.85546875" customWidth="1"/>
+    <col min="136" max="158" width="10.81640625" customWidth="1"/>
+    <col min="16384" max="16384" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:163 16384:16384" ht="21">
-      <c r="A1" s="128" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="128"/>
+      <c r="B1" s="89"/>
       <c r="C1" s="34"/>
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
@@ -2438,7 +2437,7 @@
       <c r="ED1" s="4"/>
       <c r="EE1" s="4"/>
     </row>
-    <row r="2" spans="1:163 16384:16384" ht="15.75" thickBot="1">
+    <row r="2" spans="1:163 16384:16384" ht="15" thickBot="1">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -2599,185 +2598,185 @@
       <c r="FB2" s="4"/>
       <c r="XFD2" s="4"/>
     </row>
-    <row r="3" spans="1:163 16384:16384" ht="15.75" thickBot="1">
+    <row r="3" spans="1:163 16384:16384" ht="15" thickBot="1">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B3" s="28">
         <f>SUM(C6:EZ6,C8:EZ8,C10:EZ10,C12:EL12,C14:EZ14,C16:EZ16,C18:EZ18,C20:EZ20,C24:EZ24,C26:EZ26,C28:EZ28,C30:EZ30,C32:EZ32,C34:EZ34,C36:EZ36)</f>
         <v>207</v>
       </c>
-      <c r="C3" s="92" t="s">
+      <c r="C3" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="91"/>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="91"/>
+      <c r="H3" s="91"/>
+      <c r="I3" s="92"/>
+      <c r="J3" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="93"/>
-      <c r="E3" s="93"/>
-      <c r="F3" s="93"/>
-      <c r="G3" s="93"/>
-      <c r="H3" s="93"/>
-      <c r="I3" s="94"/>
-      <c r="J3" s="92" t="s">
+      <c r="K3" s="91"/>
+      <c r="L3" s="91"/>
+      <c r="M3" s="91"/>
+      <c r="N3" s="91"/>
+      <c r="O3" s="91"/>
+      <c r="P3" s="92"/>
+      <c r="Q3" s="90" t="s">
         <v>73</v>
       </c>
-      <c r="K3" s="93"/>
-      <c r="L3" s="93"/>
-      <c r="M3" s="93"/>
-      <c r="N3" s="93"/>
-      <c r="O3" s="93"/>
-      <c r="P3" s="94"/>
-      <c r="Q3" s="92" t="s">
+      <c r="R3" s="91"/>
+      <c r="S3" s="91"/>
+      <c r="T3" s="91"/>
+      <c r="U3" s="91"/>
+      <c r="V3" s="91"/>
+      <c r="W3" s="92"/>
+      <c r="X3" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="R3" s="93"/>
-      <c r="S3" s="93"/>
-      <c r="T3" s="93"/>
-      <c r="U3" s="93"/>
-      <c r="V3" s="93"/>
-      <c r="W3" s="94"/>
-      <c r="X3" s="92" t="s">
+      <c r="Y3" s="91"/>
+      <c r="Z3" s="91"/>
+      <c r="AA3" s="91"/>
+      <c r="AB3" s="91"/>
+      <c r="AC3" s="91"/>
+      <c r="AD3" s="92"/>
+      <c r="AE3" s="90" t="s">
         <v>75</v>
       </c>
-      <c r="Y3" s="93"/>
-      <c r="Z3" s="93"/>
-      <c r="AA3" s="93"/>
-      <c r="AB3" s="93"/>
-      <c r="AC3" s="93"/>
-      <c r="AD3" s="94"/>
-      <c r="AE3" s="92" t="s">
+      <c r="AF3" s="91"/>
+      <c r="AG3" s="91"/>
+      <c r="AH3" s="91"/>
+      <c r="AI3" s="91"/>
+      <c r="AJ3" s="91"/>
+      <c r="AK3" s="92"/>
+      <c r="AL3" s="90" t="s">
         <v>76</v>
       </c>
-      <c r="AF3" s="93"/>
-      <c r="AG3" s="93"/>
-      <c r="AH3" s="93"/>
-      <c r="AI3" s="93"/>
-      <c r="AJ3" s="93"/>
-      <c r="AK3" s="94"/>
-      <c r="AL3" s="92" t="s">
+      <c r="AM3" s="91"/>
+      <c r="AN3" s="91"/>
+      <c r="AO3" s="91"/>
+      <c r="AP3" s="91"/>
+      <c r="AQ3" s="91"/>
+      <c r="AR3" s="92"/>
+      <c r="AS3" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="AM3" s="93"/>
-      <c r="AN3" s="93"/>
-      <c r="AO3" s="93"/>
-      <c r="AP3" s="93"/>
-      <c r="AQ3" s="93"/>
-      <c r="AR3" s="94"/>
-      <c r="AS3" s="92" t="s">
+      <c r="AT3" s="91"/>
+      <c r="AU3" s="91"/>
+      <c r="AV3" s="91"/>
+      <c r="AW3" s="91"/>
+      <c r="AX3" s="91"/>
+      <c r="AY3" s="92"/>
+      <c r="AZ3" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="AT3" s="93"/>
-      <c r="AU3" s="93"/>
-      <c r="AV3" s="93"/>
-      <c r="AW3" s="93"/>
-      <c r="AX3" s="93"/>
-      <c r="AY3" s="94"/>
-      <c r="AZ3" s="92" t="s">
+      <c r="BA3" s="91"/>
+      <c r="BB3" s="91"/>
+      <c r="BC3" s="91"/>
+      <c r="BD3" s="91"/>
+      <c r="BE3" s="91"/>
+      <c r="BF3" s="92"/>
+      <c r="BG3" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="BA3" s="93"/>
-      <c r="BB3" s="93"/>
-      <c r="BC3" s="93"/>
-      <c r="BD3" s="93"/>
-      <c r="BE3" s="93"/>
-      <c r="BF3" s="94"/>
-      <c r="BG3" s="92" t="s">
+      <c r="BH3" s="91"/>
+      <c r="BI3" s="91"/>
+      <c r="BJ3" s="91"/>
+      <c r="BK3" s="91"/>
+      <c r="BL3" s="91"/>
+      <c r="BM3" s="92"/>
+      <c r="BN3" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="BH3" s="93"/>
-      <c r="BI3" s="93"/>
-      <c r="BJ3" s="93"/>
-      <c r="BK3" s="93"/>
-      <c r="BL3" s="93"/>
-      <c r="BM3" s="94"/>
-      <c r="BN3" s="92" t="s">
+      <c r="BO3" s="91"/>
+      <c r="BP3" s="91"/>
+      <c r="BQ3" s="91"/>
+      <c r="BR3" s="91"/>
+      <c r="BS3" s="91"/>
+      <c r="BT3" s="92"/>
+      <c r="BU3" s="90" t="s">
         <v>81</v>
       </c>
-      <c r="BO3" s="93"/>
-      <c r="BP3" s="93"/>
-      <c r="BQ3" s="93"/>
-      <c r="BR3" s="93"/>
-      <c r="BS3" s="93"/>
-      <c r="BT3" s="94"/>
-      <c r="BU3" s="92" t="s">
+      <c r="BV3" s="91"/>
+      <c r="BW3" s="91"/>
+      <c r="BX3" s="91"/>
+      <c r="BY3" s="91"/>
+      <c r="BZ3" s="91"/>
+      <c r="CA3" s="92"/>
+      <c r="CB3" s="90" t="s">
         <v>82</v>
       </c>
-      <c r="BV3" s="93"/>
-      <c r="BW3" s="93"/>
-      <c r="BX3" s="93"/>
-      <c r="BY3" s="93"/>
-      <c r="BZ3" s="93"/>
-      <c r="CA3" s="94"/>
-      <c r="CB3" s="92" t="s">
+      <c r="CC3" s="91"/>
+      <c r="CD3" s="91"/>
+      <c r="CE3" s="91"/>
+      <c r="CF3" s="91"/>
+      <c r="CG3" s="91"/>
+      <c r="CH3" s="92"/>
+      <c r="CI3" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="CC3" s="93"/>
-      <c r="CD3" s="93"/>
-      <c r="CE3" s="93"/>
-      <c r="CF3" s="93"/>
-      <c r="CG3" s="93"/>
-      <c r="CH3" s="94"/>
-      <c r="CI3" s="92" t="s">
+      <c r="CJ3" s="91"/>
+      <c r="CK3" s="91"/>
+      <c r="CL3" s="91"/>
+      <c r="CM3" s="91"/>
+      <c r="CN3" s="91"/>
+      <c r="CO3" s="92"/>
+      <c r="CP3" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="CJ3" s="93"/>
-      <c r="CK3" s="93"/>
-      <c r="CL3" s="93"/>
-      <c r="CM3" s="93"/>
-      <c r="CN3" s="93"/>
-      <c r="CO3" s="94"/>
-      <c r="CP3" s="92" t="s">
+      <c r="CQ3" s="91"/>
+      <c r="CR3" s="91"/>
+      <c r="CS3" s="91"/>
+      <c r="CT3" s="91"/>
+      <c r="CU3" s="91"/>
+      <c r="CV3" s="92"/>
+      <c r="CW3" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="CQ3" s="93"/>
-      <c r="CR3" s="93"/>
-      <c r="CS3" s="93"/>
-      <c r="CT3" s="93"/>
-      <c r="CU3" s="93"/>
-      <c r="CV3" s="94"/>
-      <c r="CW3" s="92" t="s">
+      <c r="CX3" s="91"/>
+      <c r="CY3" s="91"/>
+      <c r="CZ3" s="91"/>
+      <c r="DA3" s="91"/>
+      <c r="DB3" s="91"/>
+      <c r="DC3" s="92"/>
+      <c r="DD3" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="CX3" s="93"/>
-      <c r="CY3" s="93"/>
-      <c r="CZ3" s="93"/>
-      <c r="DA3" s="93"/>
-      <c r="DB3" s="93"/>
-      <c r="DC3" s="94"/>
-      <c r="DD3" s="92" t="s">
+      <c r="DE3" s="91"/>
+      <c r="DF3" s="91"/>
+      <c r="DG3" s="91"/>
+      <c r="DH3" s="91"/>
+      <c r="DI3" s="91"/>
+      <c r="DJ3" s="92"/>
+      <c r="DK3" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="DE3" s="93"/>
-      <c r="DF3" s="93"/>
-      <c r="DG3" s="93"/>
-      <c r="DH3" s="93"/>
-      <c r="DI3" s="93"/>
-      <c r="DJ3" s="94"/>
-      <c r="DK3" s="92" t="s">
+      <c r="DL3" s="91"/>
+      <c r="DM3" s="91"/>
+      <c r="DN3" s="91"/>
+      <c r="DO3" s="91"/>
+      <c r="DP3" s="91"/>
+      <c r="DQ3" s="92"/>
+      <c r="DR3" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="DL3" s="93"/>
-      <c r="DM3" s="93"/>
-      <c r="DN3" s="93"/>
-      <c r="DO3" s="93"/>
-      <c r="DP3" s="93"/>
-      <c r="DQ3" s="94"/>
-      <c r="DR3" s="92" t="s">
+      <c r="DS3" s="91"/>
+      <c r="DT3" s="91"/>
+      <c r="DU3" s="91"/>
+      <c r="DV3" s="91"/>
+      <c r="DW3" s="91"/>
+      <c r="DX3" s="92"/>
+      <c r="DY3" s="93" t="s">
         <v>89</v>
       </c>
-      <c r="DS3" s="93"/>
-      <c r="DT3" s="93"/>
-      <c r="DU3" s="93"/>
-      <c r="DV3" s="93"/>
-      <c r="DW3" s="93"/>
-      <c r="DX3" s="94"/>
-      <c r="DY3" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="DZ3" s="123"/>
-      <c r="EA3" s="123"/>
-      <c r="EB3" s="123"/>
-      <c r="EC3" s="123"/>
-      <c r="ED3" s="123"/>
-      <c r="EE3" s="124"/>
+      <c r="DZ3" s="94"/>
+      <c r="EA3" s="94"/>
+      <c r="EB3" s="94"/>
+      <c r="EC3" s="94"/>
+      <c r="ED3" s="94"/>
+      <c r="EE3" s="95"/>
       <c r="EF3" s="74"/>
       <c r="EG3" s="74"/>
       <c r="EH3" s="74"/>
@@ -2800,9 +2799,9 @@
       <c r="EY3" s="74"/>
       <c r="EZ3" s="74"/>
     </row>
-    <row r="4" spans="1:163 16384:16384" ht="15.75" thickBot="1">
+    <row r="4" spans="1:163 16384:16384" ht="15" thickBot="1">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B4" s="25">
         <f>SUM(C7:EZ7,C9:EZ9,C11:EZ11,C13:EZ13,C15:EZ15,C17:EZ17,C19:EZ19,C21:EZ21,C23:EZ23,C25:EZ25,C27:EZ27,C29:EZ29,C31:EZ31,C33:EZ33,C35:EZ35,C37:EZ37)</f>
@@ -3232,144 +3231,144 @@
       <c r="FB4" s="69"/>
       <c r="XFD4" s="69"/>
     </row>
-    <row r="5" spans="1:163 16384:16384" ht="19.5" thickBot="1">
-      <c r="A5" s="102" t="s">
-        <v>53</v>
-      </c>
-      <c r="B5" s="103"/>
-      <c r="C5" s="95"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="96"/>
-      <c r="F5" s="96"/>
-      <c r="G5" s="96"/>
-      <c r="H5" s="96"/>
-      <c r="I5" s="97"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="96"/>
-      <c r="L5" s="96"/>
-      <c r="M5" s="96"/>
-      <c r="N5" s="96"/>
-      <c r="O5" s="96"/>
-      <c r="P5" s="97"/>
-      <c r="Q5" s="95"/>
-      <c r="R5" s="96"/>
-      <c r="S5" s="96"/>
-      <c r="T5" s="96"/>
-      <c r="U5" s="96"/>
-      <c r="V5" s="96"/>
-      <c r="W5" s="97"/>
-      <c r="X5" s="105"/>
-      <c r="Y5" s="105"/>
-      <c r="Z5" s="105"/>
-      <c r="AA5" s="105"/>
-      <c r="AB5" s="105"/>
-      <c r="AC5" s="105"/>
-      <c r="AD5" s="106"/>
-      <c r="AE5" s="107"/>
-      <c r="AF5" s="105"/>
-      <c r="AG5" s="105"/>
-      <c r="AH5" s="105"/>
-      <c r="AI5" s="105"/>
-      <c r="AJ5" s="105"/>
-      <c r="AK5" s="106"/>
-      <c r="AL5" s="108"/>
-      <c r="AM5" s="109"/>
-      <c r="AN5" s="109"/>
-      <c r="AO5" s="109"/>
-      <c r="AP5" s="109"/>
-      <c r="AQ5" s="109"/>
-      <c r="AR5" s="110"/>
-      <c r="AS5" s="107"/>
-      <c r="AT5" s="105"/>
-      <c r="AU5" s="105"/>
-      <c r="AV5" s="105"/>
-      <c r="AW5" s="105"/>
-      <c r="AX5" s="105"/>
-      <c r="AY5" s="106"/>
-      <c r="AZ5" s="119"/>
-      <c r="BA5" s="120"/>
-      <c r="BB5" s="120"/>
-      <c r="BC5" s="120"/>
-      <c r="BD5" s="120"/>
-      <c r="BE5" s="120"/>
-      <c r="BF5" s="121"/>
-      <c r="BG5" s="107"/>
-      <c r="BH5" s="105"/>
-      <c r="BI5" s="105"/>
-      <c r="BJ5" s="105"/>
-      <c r="BK5" s="105"/>
-      <c r="BL5" s="105"/>
-      <c r="BM5" s="106"/>
-      <c r="BN5" s="107"/>
-      <c r="BO5" s="105"/>
-      <c r="BP5" s="105"/>
-      <c r="BQ5" s="105"/>
-      <c r="BR5" s="105"/>
-      <c r="BS5" s="105"/>
-      <c r="BT5" s="106"/>
-      <c r="BU5" s="107"/>
-      <c r="BV5" s="105"/>
-      <c r="BW5" s="105"/>
-      <c r="BX5" s="105"/>
-      <c r="BY5" s="105"/>
-      <c r="BZ5" s="105"/>
-      <c r="CA5" s="106"/>
-      <c r="CB5" s="107"/>
-      <c r="CC5" s="105"/>
-      <c r="CD5" s="105"/>
-      <c r="CE5" s="105"/>
-      <c r="CF5" s="105"/>
-      <c r="CG5" s="105"/>
-      <c r="CH5" s="106"/>
-      <c r="CI5" s="107"/>
-      <c r="CJ5" s="105"/>
-      <c r="CK5" s="105"/>
-      <c r="CL5" s="105"/>
-      <c r="CM5" s="105"/>
-      <c r="CN5" s="105"/>
-      <c r="CO5" s="106"/>
-      <c r="CP5" s="107"/>
-      <c r="CQ5" s="105"/>
-      <c r="CR5" s="105"/>
-      <c r="CS5" s="105"/>
-      <c r="CT5" s="105"/>
-      <c r="CU5" s="105"/>
-      <c r="CV5" s="106"/>
-      <c r="CW5" s="107"/>
-      <c r="CX5" s="105"/>
-      <c r="CY5" s="105"/>
-      <c r="CZ5" s="105"/>
-      <c r="DA5" s="105"/>
-      <c r="DB5" s="105"/>
-      <c r="DC5" s="106"/>
-      <c r="DD5" s="107"/>
-      <c r="DE5" s="105"/>
-      <c r="DF5" s="105"/>
-      <c r="DG5" s="105"/>
-      <c r="DH5" s="105"/>
-      <c r="DI5" s="105"/>
-      <c r="DJ5" s="106"/>
-      <c r="DK5" s="107"/>
-      <c r="DL5" s="105"/>
-      <c r="DM5" s="105"/>
-      <c r="DN5" s="105"/>
-      <c r="DO5" s="105"/>
-      <c r="DP5" s="105"/>
-      <c r="DQ5" s="106"/>
-      <c r="DR5" s="107"/>
-      <c r="DS5" s="105"/>
-      <c r="DT5" s="105"/>
-      <c r="DU5" s="105"/>
-      <c r="DV5" s="105"/>
-      <c r="DW5" s="105"/>
-      <c r="DX5" s="106"/>
-      <c r="DY5" s="125"/>
-      <c r="DZ5" s="126"/>
-      <c r="EA5" s="126"/>
-      <c r="EB5" s="126"/>
-      <c r="EC5" s="126"/>
-      <c r="ED5" s="126"/>
-      <c r="EE5" s="127"/>
+    <row r="5" spans="1:163 16384:16384" ht="19" thickBot="1">
+      <c r="A5" s="126" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="127"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="115"/>
+      <c r="E5" s="115"/>
+      <c r="F5" s="115"/>
+      <c r="G5" s="115"/>
+      <c r="H5" s="115"/>
+      <c r="I5" s="116"/>
+      <c r="J5" s="114"/>
+      <c r="K5" s="115"/>
+      <c r="L5" s="115"/>
+      <c r="M5" s="115"/>
+      <c r="N5" s="115"/>
+      <c r="O5" s="115"/>
+      <c r="P5" s="116"/>
+      <c r="Q5" s="114"/>
+      <c r="R5" s="115"/>
+      <c r="S5" s="115"/>
+      <c r="T5" s="115"/>
+      <c r="U5" s="115"/>
+      <c r="V5" s="115"/>
+      <c r="W5" s="116"/>
+      <c r="X5" s="97"/>
+      <c r="Y5" s="97"/>
+      <c r="Z5" s="97"/>
+      <c r="AA5" s="97"/>
+      <c r="AB5" s="97"/>
+      <c r="AC5" s="97"/>
+      <c r="AD5" s="98"/>
+      <c r="AE5" s="96"/>
+      <c r="AF5" s="97"/>
+      <c r="AG5" s="97"/>
+      <c r="AH5" s="97"/>
+      <c r="AI5" s="97"/>
+      <c r="AJ5" s="97"/>
+      <c r="AK5" s="98"/>
+      <c r="AL5" s="117"/>
+      <c r="AM5" s="118"/>
+      <c r="AN5" s="118"/>
+      <c r="AO5" s="118"/>
+      <c r="AP5" s="118"/>
+      <c r="AQ5" s="118"/>
+      <c r="AR5" s="119"/>
+      <c r="AS5" s="96"/>
+      <c r="AT5" s="97"/>
+      <c r="AU5" s="97"/>
+      <c r="AV5" s="97"/>
+      <c r="AW5" s="97"/>
+      <c r="AX5" s="97"/>
+      <c r="AY5" s="98"/>
+      <c r="AZ5" s="111"/>
+      <c r="BA5" s="112"/>
+      <c r="BB5" s="112"/>
+      <c r="BC5" s="112"/>
+      <c r="BD5" s="112"/>
+      <c r="BE5" s="112"/>
+      <c r="BF5" s="113"/>
+      <c r="BG5" s="96"/>
+      <c r="BH5" s="97"/>
+      <c r="BI5" s="97"/>
+      <c r="BJ5" s="97"/>
+      <c r="BK5" s="97"/>
+      <c r="BL5" s="97"/>
+      <c r="BM5" s="98"/>
+      <c r="BN5" s="96"/>
+      <c r="BO5" s="97"/>
+      <c r="BP5" s="97"/>
+      <c r="BQ5" s="97"/>
+      <c r="BR5" s="97"/>
+      <c r="BS5" s="97"/>
+      <c r="BT5" s="98"/>
+      <c r="BU5" s="96"/>
+      <c r="BV5" s="97"/>
+      <c r="BW5" s="97"/>
+      <c r="BX5" s="97"/>
+      <c r="BY5" s="97"/>
+      <c r="BZ5" s="97"/>
+      <c r="CA5" s="98"/>
+      <c r="CB5" s="96"/>
+      <c r="CC5" s="97"/>
+      <c r="CD5" s="97"/>
+      <c r="CE5" s="97"/>
+      <c r="CF5" s="97"/>
+      <c r="CG5" s="97"/>
+      <c r="CH5" s="98"/>
+      <c r="CI5" s="96"/>
+      <c r="CJ5" s="97"/>
+      <c r="CK5" s="97"/>
+      <c r="CL5" s="97"/>
+      <c r="CM5" s="97"/>
+      <c r="CN5" s="97"/>
+      <c r="CO5" s="98"/>
+      <c r="CP5" s="96"/>
+      <c r="CQ5" s="97"/>
+      <c r="CR5" s="97"/>
+      <c r="CS5" s="97"/>
+      <c r="CT5" s="97"/>
+      <c r="CU5" s="97"/>
+      <c r="CV5" s="98"/>
+      <c r="CW5" s="96"/>
+      <c r="CX5" s="97"/>
+      <c r="CY5" s="97"/>
+      <c r="CZ5" s="97"/>
+      <c r="DA5" s="97"/>
+      <c r="DB5" s="97"/>
+      <c r="DC5" s="98"/>
+      <c r="DD5" s="96"/>
+      <c r="DE5" s="97"/>
+      <c r="DF5" s="97"/>
+      <c r="DG5" s="97"/>
+      <c r="DH5" s="97"/>
+      <c r="DI5" s="97"/>
+      <c r="DJ5" s="98"/>
+      <c r="DK5" s="96"/>
+      <c r="DL5" s="97"/>
+      <c r="DM5" s="97"/>
+      <c r="DN5" s="97"/>
+      <c r="DO5" s="97"/>
+      <c r="DP5" s="97"/>
+      <c r="DQ5" s="98"/>
+      <c r="DR5" s="96"/>
+      <c r="DS5" s="97"/>
+      <c r="DT5" s="97"/>
+      <c r="DU5" s="97"/>
+      <c r="DV5" s="97"/>
+      <c r="DW5" s="97"/>
+      <c r="DX5" s="98"/>
+      <c r="DY5" s="99"/>
+      <c r="DZ5" s="100"/>
+      <c r="EA5" s="100"/>
+      <c r="EB5" s="100"/>
+      <c r="EC5" s="100"/>
+      <c r="ED5" s="100"/>
+      <c r="EE5" s="101"/>
       <c r="EF5" s="73"/>
       <c r="EG5" s="73"/>
       <c r="EH5" s="73"/>
@@ -3400,7 +3399,7 @@
       <c r="FG5" s="1"/>
     </row>
     <row r="6" spans="1:163 16384:16384" ht="15" customHeight="1" thickBot="1">
-      <c r="A6" s="104" t="s">
+      <c r="A6" s="128" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -3607,7 +3606,7 @@
       <c r="XFD6" s="70"/>
     </row>
     <row r="7" spans="1:163 16384:16384" ht="15" customHeight="1" thickBot="1">
-      <c r="A7" s="90"/>
+      <c r="A7" s="122"/>
       <c r="B7" s="27" t="s">
         <v>10</v>
       </c>
@@ -3770,8 +3769,8 @@
       <c r="XFD7" s="71"/>
     </row>
     <row r="8" spans="1:163 16384:16384" ht="15" customHeight="1" thickBot="1">
-      <c r="A8" s="98" t="s">
-        <v>91</v>
+      <c r="A8" s="124" t="s">
+        <v>90</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>9</v>
@@ -3945,7 +3944,7 @@
       <c r="XFD8" s="71"/>
     </row>
     <row r="9" spans="1:163 16384:16384" ht="15" customHeight="1" thickBot="1">
-      <c r="A9" s="99"/>
+      <c r="A9" s="125"/>
       <c r="B9" s="37" t="s">
         <v>10</v>
       </c>
@@ -4103,9 +4102,9 @@
       <c r="FB9" s="71"/>
       <c r="XFD9" s="71"/>
     </row>
-    <row r="10" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A10" s="100" t="s">
-        <v>52</v>
+    <row r="10" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A10" s="102" t="s">
+        <v>51</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>9</v>
@@ -4269,8 +4268,8 @@
       <c r="FB10" s="71"/>
       <c r="XFD10" s="71"/>
     </row>
-    <row r="11" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A11" s="101"/>
+    <row r="11" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A11" s="103"/>
       <c r="B11" s="27" t="s">
         <v>10</v>
       </c>
@@ -4436,8 +4435,8 @@
       <c r="FB11" s="71"/>
       <c r="XFD11" s="71"/>
     </row>
-    <row r="12" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A12" s="111" t="s">
+    <row r="12" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A12" s="106" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="26" t="s">
@@ -4604,8 +4603,8 @@
       <c r="FB12" s="71"/>
       <c r="XFD12" s="71"/>
     </row>
-    <row r="13" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A13" s="112"/>
+    <row r="13" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A13" s="120"/>
       <c r="B13" s="27" t="s">
         <v>10</v>
       </c>
@@ -4773,8 +4772,8 @@
       <c r="FB13" s="71"/>
       <c r="XFD13" s="71"/>
     </row>
-    <row r="14" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A14" s="100" t="s">
+    <row r="14" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A14" s="102" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="26" t="s">
@@ -4942,8 +4941,8 @@
       <c r="FB14" s="71"/>
       <c r="XFD14" s="71"/>
     </row>
-    <row r="15" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A15" s="101"/>
+    <row r="15" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A15" s="103"/>
       <c r="B15" s="27" t="s">
         <v>10</v>
       </c>
@@ -5114,9 +5113,9 @@
       <c r="FB15" s="71"/>
       <c r="XFD15" s="71"/>
     </row>
-    <row r="16" spans="1:163 16384:16384" ht="15.75" thickBot="1">
-      <c r="A16" s="111" t="s">
-        <v>56</v>
+    <row r="16" spans="1:163 16384:16384" ht="15" thickBot="1">
+      <c r="A16" s="106" t="s">
+        <v>55</v>
       </c>
       <c r="B16" s="26" t="s">
         <v>9</v>
@@ -5279,8 +5278,8 @@
       <c r="FB16" s="71"/>
       <c r="XFD16" s="71"/>
     </row>
-    <row r="17" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A17" s="115"/>
+    <row r="17" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A17" s="107"/>
       <c r="B17" s="27" t="s">
         <v>10</v>
       </c>
@@ -5444,9 +5443,9 @@
       <c r="FB17" s="71"/>
       <c r="XFD17" s="71"/>
     </row>
-    <row r="18" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A18" s="111" t="s">
-        <v>92</v>
+    <row r="18" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A18" s="106" t="s">
+        <v>91</v>
       </c>
       <c r="B18" s="26" t="s">
         <v>9</v>
@@ -5610,8 +5609,8 @@
       <c r="FB18" s="71"/>
       <c r="XFD18" s="71"/>
     </row>
-    <row r="19" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A19" s="115"/>
+    <row r="19" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A19" s="107"/>
       <c r="B19" s="27" t="s">
         <v>10</v>
       </c>
@@ -5669,7 +5668,7 @@
       <c r="AX19" s="57"/>
       <c r="AY19" s="61"/>
       <c r="AZ19" s="60"/>
-      <c r="BA19" s="138"/>
+      <c r="BA19" s="57"/>
       <c r="BB19" s="87">
         <v>4</v>
       </c>
@@ -5783,9 +5782,9 @@
       <c r="FB19" s="71"/>
       <c r="XFD19" s="71"/>
     </row>
-    <row r="20" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A20" s="89" t="s">
-        <v>93</v>
+    <row r="20" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A20" s="121" t="s">
+        <v>92</v>
       </c>
       <c r="B20" s="26" t="s">
         <v>9</v>
@@ -5856,7 +5855,7 @@
       <c r="BL20" s="57"/>
       <c r="BM20" s="61"/>
       <c r="BN20" s="60"/>
-      <c r="BO20" s="138"/>
+      <c r="BO20" s="57"/>
       <c r="BP20" s="57"/>
       <c r="BQ20" s="57"/>
       <c r="BR20" s="57"/>
@@ -5950,8 +5949,8 @@
       <c r="FB20" s="71"/>
       <c r="XFD20" s="71"/>
     </row>
-    <row r="21" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A21" s="90"/>
+    <row r="21" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A21" s="122"/>
       <c r="B21" s="27" t="s">
         <v>10</v>
       </c>
@@ -6115,9 +6114,9 @@
       <c r="FB21" s="71"/>
       <c r="XFD21" s="71"/>
     </row>
-    <row r="22" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A22" s="89" t="s">
-        <v>94</v>
+    <row r="22" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A22" s="121" t="s">
+        <v>93</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>9</v>
@@ -6281,8 +6280,8 @@
       <c r="FB22" s="71"/>
       <c r="XFD22" s="71"/>
     </row>
-    <row r="23" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A23" s="91"/>
+    <row r="23" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A23" s="123"/>
       <c r="B23" s="27" t="s">
         <v>10</v>
       </c>
@@ -6443,9 +6442,9 @@
       <c r="FB23" s="71"/>
       <c r="XFD23" s="71"/>
     </row>
-    <row r="24" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A24" s="100" t="s">
-        <v>47</v>
+    <row r="24" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A24" s="102" t="s">
+        <v>46</v>
       </c>
       <c r="B24" s="26" t="s">
         <v>9</v>
@@ -6615,8 +6614,8 @@
       <c r="FB24" s="71"/>
       <c r="XFD24" s="71"/>
     </row>
-    <row r="25" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A25" s="101"/>
+    <row r="25" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A25" s="103"/>
       <c r="B25" s="27" t="s">
         <v>10</v>
       </c>
@@ -6778,9 +6777,9 @@
       <c r="FB25" s="71"/>
       <c r="XFD25" s="71"/>
     </row>
-    <row r="26" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A26" s="116" t="s">
-        <v>48</v>
+    <row r="26" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A26" s="108" t="s">
+        <v>47</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>9</v>
@@ -6941,8 +6940,8 @@
       <c r="FB26" s="71"/>
       <c r="XFD26" s="71"/>
     </row>
-    <row r="27" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A27" s="117"/>
+    <row r="27" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A27" s="109"/>
       <c r="B27" s="27" t="s">
         <v>10</v>
       </c>
@@ -7104,9 +7103,9 @@
       <c r="FB27" s="71"/>
       <c r="XFD27" s="71"/>
     </row>
-    <row r="28" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A28" s="116" t="s">
-        <v>55</v>
+    <row r="28" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A28" s="108" t="s">
+        <v>54</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>9</v>
@@ -7269,8 +7268,8 @@
       <c r="FB28" s="71"/>
       <c r="XFD28" s="71"/>
     </row>
-    <row r="29" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A29" s="118"/>
+    <row r="29" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A29" s="110"/>
       <c r="B29" s="27" t="s">
         <v>10</v>
       </c>
@@ -7432,9 +7431,9 @@
       <c r="FB29" s="71"/>
       <c r="XFD29" s="71"/>
     </row>
-    <row r="30" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A30" s="100" t="s">
-        <v>49</v>
+    <row r="30" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A30" s="102" t="s">
+        <v>48</v>
       </c>
       <c r="B30" s="26" t="s">
         <v>9</v>
@@ -7663,8 +7662,8 @@
       <c r="FB30" s="71"/>
       <c r="XFD30" s="71"/>
     </row>
-    <row r="31" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A31" s="101"/>
+    <row r="31" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A31" s="103"/>
       <c r="B31" s="27" t="s">
         <v>10</v>
       </c>
@@ -7826,9 +7825,9 @@
       <c r="FB31" s="71"/>
       <c r="XFD31" s="71"/>
     </row>
-    <row r="32" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A32" s="100" t="s">
-        <v>50</v>
+    <row r="32" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A32" s="102" t="s">
+        <v>49</v>
       </c>
       <c r="B32" s="26" t="s">
         <v>9</v>
@@ -7999,8 +7998,8 @@
       <c r="FB32" s="71"/>
       <c r="XFD32" s="71"/>
     </row>
-    <row r="33" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A33" s="113"/>
+    <row r="33" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A33" s="104"/>
       <c r="B33" s="27" t="s">
         <v>10</v>
       </c>
@@ -8162,8 +8161,8 @@
       <c r="FB33" s="71"/>
       <c r="XFD33" s="71"/>
     </row>
-    <row r="34" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A34" s="100" t="s">
+    <row r="34" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A34" s="102" t="s">
         <v>12</v>
       </c>
       <c r="B34" s="26" t="s">
@@ -8335,8 +8334,8 @@
       <c r="FB34" s="71"/>
       <c r="XFD34" s="71"/>
     </row>
-    <row r="35" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A35" s="101"/>
+    <row r="35" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A35" s="103"/>
       <c r="B35" s="27" t="s">
         <v>10</v>
       </c>
@@ -8498,9 +8497,9 @@
       <c r="FB35" s="71"/>
       <c r="XFD35" s="71"/>
     </row>
-    <row r="36" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A36" s="100" t="s">
-        <v>51</v>
+    <row r="36" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A36" s="102" t="s">
+        <v>50</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>9</v>
@@ -8665,8 +8664,8 @@
       <c r="FB36" s="71"/>
       <c r="XFD36" s="71"/>
     </row>
-    <row r="37" spans="1:158 16384:16384" ht="15.75" thickBot="1">
-      <c r="A37" s="114"/>
+    <row r="37" spans="1:158 16384:16384" ht="15" thickBot="1">
+      <c r="A37" s="105"/>
       <c r="B37" s="27" t="s">
         <v>10</v>
       </c>
@@ -8830,30 +8829,22 @@
     </row>
   </sheetData>
   <mergeCells count="56">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="X3:AD3"/>
-    <mergeCell ref="AE3:AK3"/>
-    <mergeCell ref="AL3:AR3"/>
-    <mergeCell ref="DR3:DX3"/>
-    <mergeCell ref="DY3:EE3"/>
-    <mergeCell ref="CI5:CO5"/>
-    <mergeCell ref="CP5:CV5"/>
-    <mergeCell ref="CW5:DC5"/>
-    <mergeCell ref="DD5:DJ5"/>
-    <mergeCell ref="DK5:DQ5"/>
-    <mergeCell ref="CP3:CV3"/>
-    <mergeCell ref="CW3:DC3"/>
-    <mergeCell ref="DD3:DJ3"/>
-    <mergeCell ref="DK3:DQ3"/>
-    <mergeCell ref="CI3:CO3"/>
-    <mergeCell ref="DR5:DX5"/>
-    <mergeCell ref="DY5:EE5"/>
-    <mergeCell ref="AS3:AY3"/>
-    <mergeCell ref="AZ3:BF3"/>
-    <mergeCell ref="BG3:BM3"/>
-    <mergeCell ref="BN3:BT3"/>
-    <mergeCell ref="BU3:CA3"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="J3:P3"/>
+    <mergeCell ref="J5:P5"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C5:I5"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="X5:AD5"/>
+    <mergeCell ref="AE5:AK5"/>
+    <mergeCell ref="AL5:AR5"/>
+    <mergeCell ref="AS5:AY5"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A12:A13"/>
     <mergeCell ref="CB3:CH3"/>
     <mergeCell ref="A30:A31"/>
     <mergeCell ref="A32:A33"/>
@@ -8870,22 +8861,30 @@
     <mergeCell ref="BU5:CA5"/>
     <mergeCell ref="CB5:CH5"/>
     <mergeCell ref="Q5:W5"/>
-    <mergeCell ref="X5:AD5"/>
-    <mergeCell ref="AE5:AK5"/>
-    <mergeCell ref="AL5:AR5"/>
-    <mergeCell ref="AS5:AY5"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="J3:P3"/>
-    <mergeCell ref="J5:P5"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C5:I5"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="AS3:AY3"/>
+    <mergeCell ref="AZ3:BF3"/>
+    <mergeCell ref="BG3:BM3"/>
+    <mergeCell ref="BN3:BT3"/>
+    <mergeCell ref="BU3:CA3"/>
+    <mergeCell ref="DR3:DX3"/>
+    <mergeCell ref="DY3:EE3"/>
+    <mergeCell ref="CI5:CO5"/>
+    <mergeCell ref="CP5:CV5"/>
+    <mergeCell ref="CW5:DC5"/>
+    <mergeCell ref="DD5:DJ5"/>
+    <mergeCell ref="DK5:DQ5"/>
+    <mergeCell ref="CP3:CV3"/>
+    <mergeCell ref="CW3:DC3"/>
+    <mergeCell ref="DD3:DJ3"/>
+    <mergeCell ref="DK3:DQ3"/>
+    <mergeCell ref="CI3:CO3"/>
+    <mergeCell ref="DR5:DX5"/>
+    <mergeCell ref="DY5:EE5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="X3:AD3"/>
+    <mergeCell ref="AE3:AK3"/>
+    <mergeCell ref="AL3:AR3"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8897,18 +8896,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FF6EFD-F608-4DA6-AB00-E35874012156}">
   <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="43" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="72" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="94.140625" customWidth="1"/>
-    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="94.1796875" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5">
+    <row r="1" spans="1:5" ht="19">
       <c r="A1" s="129" t="s">
         <v>14</v>
       </c>
@@ -8940,7 +8939,7 @@
         <v>18</v>
       </c>
       <c r="B5" s="130" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C5" s="130"/>
       <c r="D5" s="22"/>
@@ -8986,7 +8985,7 @@
         <v>23</v>
       </c>
       <c r="B10" s="131" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="131"/>
       <c r="D10" s="131"/>
@@ -9012,8 +9011,8 @@
       <c r="C13" s="131"/>
       <c r="D13" s="22"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1"/>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+    <row r="14" spans="1:5" ht="15" thickBot="1"/>
+    <row r="15" spans="1:5" ht="15" thickBot="1">
       <c r="A15" s="32" t="s">
         <v>25</v>
       </c>
@@ -9029,10 +9028,10 @@
         <v>1</v>
       </c>
       <c r="B16" s="16" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="1:8">
@@ -9040,21 +9039,21 @@
         <v>2</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C17" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="30">
+    <row r="18" spans="1:8">
       <c r="A18" s="11">
         <v>3</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:8">
@@ -9062,10 +9061,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C19" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:8">
@@ -9073,10 +9072,10 @@
         <v>5</v>
       </c>
       <c r="B20" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D20" s="22"/>
       <c r="E20" s="22"/>
@@ -9089,10 +9088,10 @@
         <v>6</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D21" s="47"/>
       <c r="E21" s="22"/>
@@ -9105,10 +9104,10 @@
         <v>7</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D22" s="22"/>
       <c r="E22" s="22"/>
@@ -9121,10 +9120,10 @@
         <v>9</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C23" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D23" s="22"/>
       <c r="E23" s="22"/>
@@ -9137,10 +9136,10 @@
         <v>10</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D24" s="22"/>
       <c r="E24" s="22"/>
@@ -9148,15 +9147,15 @@
       <c r="G24" s="22"/>
       <c r="H24" s="22"/>
     </row>
-    <row r="25" spans="1:8" ht="30">
+    <row r="25" spans="1:8" ht="29">
       <c r="A25" s="79">
         <v>11</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D25" s="22"/>
       <c r="E25" s="22"/>
@@ -9164,15 +9163,15 @@
       <c r="G25" s="22"/>
       <c r="H25" s="22"/>
     </row>
-    <row r="26" spans="1:8" ht="14.45" customHeight="1">
+    <row r="26" spans="1:8" ht="14.5" customHeight="1">
       <c r="A26" s="80">
         <v>12</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D26" s="45"/>
       <c r="E26" s="46"/>
@@ -9185,10 +9184,10 @@
         <v>13</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C27" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D27" s="22"/>
       <c r="E27" s="22"/>
@@ -9201,10 +9200,10 @@
         <v>14</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="22"/>
@@ -9217,10 +9216,10 @@
         <v>15</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C29" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="22"/>
@@ -9234,7 +9233,7 @@
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:8">
@@ -9243,7 +9242,7 @@
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="32" spans="1:8">
@@ -9252,7 +9251,7 @@
       </c>
       <c r="B32" s="10"/>
       <c r="C32" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -9261,27 +9260,27 @@
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="15.75" thickBot="1">
+    <row r="34" spans="1:3" ht="15" thickBot="1">
       <c r="A34" s="80">
         <v>20</v>
       </c>
       <c r="B34" s="81"/>
       <c r="C34" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="131" t="s">
-        <v>28</v>
+        <v>94</v>
       </c>
       <c r="B38" s="131"/>
       <c r="C38" s="131"/>
     </row>
-    <row r="39" spans="1:3" ht="15.75" thickBot="1"/>
-    <row r="40" spans="1:3" ht="15.75" thickBot="1">
+    <row r="39" spans="1:3" ht="15" thickBot="1"/>
+    <row r="40" spans="1:3" ht="15" thickBot="1">
       <c r="A40" s="32" t="s">
         <v>25</v>
       </c>
@@ -9297,10 +9296,10 @@
         <v>1</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C41" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -9308,10 +9307,10 @@
         <v>2</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -9319,10 +9318,10 @@
         <v>3</v>
       </c>
       <c r="B43" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C43" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -9330,10 +9329,10 @@
         <v>4</v>
       </c>
       <c r="B44" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C44" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -9341,10 +9340,10 @@
         <v>5</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -9352,10 +9351,10 @@
         <v>6</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -9363,10 +9362,10 @@
         <v>7</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C47" s="39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -9376,7 +9375,7 @@
       <c r="B48" s="10"/>
       <c r="C48" s="14"/>
     </row>
-    <row r="49" spans="1:3" ht="15.75" thickBot="1">
+    <row r="49" spans="1:3" ht="15" thickBot="1">
       <c r="A49" s="13">
         <v>9</v>
       </c>
@@ -9409,21 +9408,21 @@
       <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="129.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="129.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21">
       <c r="A1" s="41" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15" thickBot="1"/>
+    <row r="3" spans="1:5" ht="15" thickBot="1">
+      <c r="A3" s="135" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="15.75" thickBot="1"/>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A3" s="135" t="s">
-        <v>57</v>
       </c>
       <c r="B3" s="136"/>
       <c r="C3" s="136"/>
@@ -9432,16 +9431,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" s="36" t="s">
         <v>58</v>
-      </c>
-      <c r="B4" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>59</v>
       </c>
       <c r="E4" s="43"/>
     </row>
@@ -9473,16 +9472,16 @@
       <c r="D8" s="57"/>
       <c r="E8" s="61"/>
     </row>
-    <row r="9" spans="1:5" ht="15.75" thickBot="1">
+    <row r="9" spans="1:5" ht="15" thickBot="1">
       <c r="A9" s="82"/>
       <c r="B9" s="83"/>
       <c r="C9" s="83"/>
       <c r="D9" s="83"/>
       <c r="E9" s="84"/>
     </row>
-    <row r="10" spans="1:5" ht="15.75" thickBot="1">
+    <row r="10" spans="1:5" ht="15" thickBot="1">
       <c r="A10" s="135" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B10" s="136"/>
       <c r="C10" s="136"/>
@@ -9491,22 +9490,22 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B11" s="36" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="43" t="s">
-        <v>59</v>
-      </c>
     </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1">
+    <row r="12" spans="1:5" ht="15" thickBot="1">
       <c r="A12" s="64"/>
       <c r="B12" s="65"/>
       <c r="C12" s="65"/>

</xml_diff>